<commit_message>
updated calibration data with new costs
</commit_message>
<xml_diff>
--- a/ref/ingestion/calibrated/argentina/model_input_variables_argentina_se_calibrated.xlsx
+++ b/ref/ingestion/calibrated/argentina/model_input_variables_argentina_se_calibrated.xlsx
@@ -603,112 +603,112 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <v>1189.63384441004</v>
+        <v>659.0425967</v>
       </c>
       <c r="K2">
-        <v>1171.912993789429</v>
+        <v>649.22546224</v>
       </c>
       <c r="L2">
-        <v>1154.192143168818</v>
+        <v>639.40832778</v>
       </c>
       <c r="M2">
-        <v>1136.471292548207</v>
+        <v>629.59119332</v>
       </c>
       <c r="N2">
-        <v>1118.750441927597</v>
+        <v>619.77405886</v>
       </c>
       <c r="O2">
-        <v>1101.029591306986</v>
+        <v>609.9569244</v>
       </c>
       <c r="P2">
-        <v>1113.073565272863</v>
+        <v>616.62913864</v>
       </c>
       <c r="Q2">
-        <v>1125.11753923874</v>
+        <v>623.30135288</v>
       </c>
       <c r="R2">
-        <v>1137.161513204616</v>
+        <v>629.97356712</v>
       </c>
       <c r="S2">
-        <v>1149.205487170493</v>
+        <v>636.64578136</v>
       </c>
       <c r="T2">
-        <v>1161.24946113637</v>
+        <v>643.3179956</v>
       </c>
       <c r="U2">
-        <v>1203.403763346923</v>
+        <v>666.67096334</v>
       </c>
       <c r="V2">
-        <v>1245.558065557477</v>
+        <v>690.02393108</v>
       </c>
       <c r="W2">
-        <v>1287.712367768031</v>
+        <v>713.37689882</v>
       </c>
       <c r="X2">
-        <v>1329.866669978584</v>
+        <v>736.72986656</v>
       </c>
       <c r="Y2">
-        <v>1372.020972189138</v>
+        <v>760.0828342999999</v>
       </c>
       <c r="Z2">
-        <v>1415.906186808908</v>
+        <v>784.39470634</v>
       </c>
       <c r="AA2">
-        <v>1459.791401428678</v>
+        <v>808.70657838</v>
       </c>
       <c r="AB2">
-        <v>1503.676616048449</v>
+        <v>833.01845042</v>
       </c>
       <c r="AC2">
-        <v>1547.561830668219</v>
+        <v>857.33032246</v>
       </c>
       <c r="AD2">
-        <v>1591.447045287989</v>
+        <v>881.6421945</v>
       </c>
       <c r="AE2">
-        <v>1635.478427864638</v>
+        <v>906.0350418</v>
       </c>
       <c r="AF2">
-        <v>1679.509810441288</v>
+        <v>930.4278891</v>
       </c>
       <c r="AG2">
-        <v>1723.541193017937</v>
+        <v>954.8207364</v>
       </c>
       <c r="AH2">
-        <v>1767.572575594586</v>
+        <v>979.2135837</v>
       </c>
       <c r="AI2">
-        <v>1811.603958171235</v>
+        <v>1003.606431</v>
       </c>
       <c r="AJ2">
-        <v>1855.174204391924</v>
+        <v>1027.7438144</v>
       </c>
       <c r="AK2">
-        <v>1898.744450612613</v>
+        <v>1051.8811978</v>
       </c>
       <c r="AL2">
-        <v>1942.314696833301</v>
+        <v>1076.0185812</v>
       </c>
       <c r="AM2">
-        <v>1985.88494305399</v>
+        <v>1100.1559646</v>
       </c>
       <c r="AN2">
-        <v>2029.455189274679</v>
+        <v>1124.293348</v>
       </c>
       <c r="AO2">
-        <v>2074.176155129041</v>
+        <v>1149.068216</v>
       </c>
       <c r="AP2">
-        <v>2118.897120983404</v>
+        <v>1173.843084</v>
       </c>
       <c r="AQ2">
-        <v>2163.618086837768</v>
+        <v>1198.617952</v>
       </c>
       <c r="AR2">
-        <v>2208.33905269213</v>
+        <v>1223.39282</v>
       </c>
       <c r="AS2">
-        <v>2253.060018546493</v>
+        <v>1248.167688</v>
       </c>
     </row>
     <row r="3" spans="1:45">
@@ -1335,112 +1335,112 @@
         <v>1</v>
       </c>
       <c r="J8">
-        <v>-0.1004827457222544</v>
+        <v>-0.1</v>
       </c>
       <c r="K8">
-        <v>-0.1004827457222544</v>
+        <v>-0.1</v>
       </c>
       <c r="L8">
-        <v>-0.1004827457222544</v>
+        <v>-0.1</v>
       </c>
       <c r="M8">
-        <v>-0.1004827457222544</v>
+        <v>-0.1</v>
       </c>
       <c r="N8">
-        <v>-0.1004827457222544</v>
+        <v>-0.1</v>
       </c>
       <c r="O8">
-        <v>-0.1004827457222544</v>
+        <v>-0.1</v>
       </c>
       <c r="P8">
-        <v>-0.1004827457222544</v>
+        <v>-0.1</v>
       </c>
       <c r="Q8">
-        <v>-0.1004827457222544</v>
+        <v>-0.1</v>
       </c>
       <c r="R8">
-        <v>-0.1004827457222544</v>
+        <v>-0.1</v>
       </c>
       <c r="S8">
-        <v>-0.1004827457222544</v>
+        <v>-0.1</v>
       </c>
       <c r="T8">
-        <v>-0.1004827457222544</v>
+        <v>-0.1</v>
       </c>
       <c r="U8">
-        <v>-0.1004827457222544</v>
+        <v>-0.1</v>
       </c>
       <c r="V8">
-        <v>-0.1004827457222544</v>
+        <v>-0.1</v>
       </c>
       <c r="W8">
-        <v>-0.1004827457222544</v>
+        <v>-0.1</v>
       </c>
       <c r="X8">
-        <v>-0.1004827457222544</v>
+        <v>-0.1</v>
       </c>
       <c r="Y8">
-        <v>-0.1004827457222544</v>
+        <v>-0.1</v>
       </c>
       <c r="Z8">
-        <v>-0.1004827457222544</v>
+        <v>-0.1</v>
       </c>
       <c r="AA8">
-        <v>-0.1004827457222544</v>
+        <v>-0.1</v>
       </c>
       <c r="AB8">
-        <v>-0.1004827457222544</v>
+        <v>-0.1</v>
       </c>
       <c r="AC8">
-        <v>-0.1004827457222544</v>
+        <v>-0.1</v>
       </c>
       <c r="AD8">
-        <v>-0.1004827457222544</v>
+        <v>-0.1</v>
       </c>
       <c r="AE8">
-        <v>-0.1004827457222544</v>
+        <v>-0.1</v>
       </c>
       <c r="AF8">
-        <v>-0.1004827457222544</v>
+        <v>-0.1</v>
       </c>
       <c r="AG8">
-        <v>-0.1004827457222544</v>
+        <v>-0.1</v>
       </c>
       <c r="AH8">
-        <v>-0.1004827457222544</v>
+        <v>-0.1</v>
       </c>
       <c r="AI8">
-        <v>-0.1004827457222544</v>
+        <v>-0.1</v>
       </c>
       <c r="AJ8">
-        <v>-0.1004827457222544</v>
+        <v>-0.1</v>
       </c>
       <c r="AK8">
-        <v>-0.1004827457222544</v>
+        <v>-0.1</v>
       </c>
       <c r="AL8">
-        <v>-0.1004827457222544</v>
+        <v>-0.1</v>
       </c>
       <c r="AM8">
-        <v>-0.1004827457222544</v>
+        <v>-0.1</v>
       </c>
       <c r="AN8">
-        <v>-0.1004827457222544</v>
+        <v>-0.1</v>
       </c>
       <c r="AO8">
-        <v>-0.1004827457222544</v>
+        <v>-0.1</v>
       </c>
       <c r="AP8">
-        <v>-0.1004827457222544</v>
+        <v>-0.1</v>
       </c>
       <c r="AQ8">
-        <v>-0.1004827457222544</v>
+        <v>-0.1</v>
       </c>
       <c r="AR8">
-        <v>-0.1004827457222544</v>
+        <v>-0.1</v>
       </c>
       <c r="AS8">
-        <v>-0.1004827457222544</v>
+        <v>-0.1</v>
       </c>
     </row>
     <row r="9" spans="1:45">
@@ -1457,112 +1457,112 @@
         <v>1</v>
       </c>
       <c r="J9">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="K9">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="L9">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="M9">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="N9">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="O9">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="P9">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="Q9">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="R9">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="S9">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="T9">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="U9">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="V9">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="W9">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="X9">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="Y9">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="Z9">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="AA9">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="AB9">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="AC9">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="AD9">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="AE9">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="AF9">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="AG9">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="AH9">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="AI9">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="AJ9">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="AK9">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="AL9">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="AM9">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="AN9">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="AO9">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="AP9">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="AQ9">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="AR9">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="AS9">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:45">
@@ -1945,112 +1945,112 @@
         <v>1</v>
       </c>
       <c r="J13">
-        <v>3.210965874462875</v>
+        <v>3.145207224</v>
       </c>
       <c r="K13">
-        <v>3.210965874462875</v>
+        <v>3.145207224</v>
       </c>
       <c r="L13">
-        <v>3.210965874462875</v>
+        <v>3.145207224</v>
       </c>
       <c r="M13">
-        <v>3.210965874462875</v>
+        <v>3.145207224</v>
       </c>
       <c r="N13">
-        <v>3.210965874462875</v>
+        <v>3.145207224</v>
       </c>
       <c r="O13">
-        <v>3.210965874462875</v>
+        <v>3.145207224</v>
       </c>
       <c r="P13">
-        <v>3.210965874462875</v>
+        <v>3.145207224</v>
       </c>
       <c r="Q13">
-        <v>3.210965874462875</v>
+        <v>3.145207224</v>
       </c>
       <c r="R13">
-        <v>3.210965874462875</v>
+        <v>3.145207224</v>
       </c>
       <c r="S13">
-        <v>3.210965874462875</v>
+        <v>3.145207224</v>
       </c>
       <c r="T13">
-        <v>3.210965874462875</v>
+        <v>3.145207224</v>
       </c>
       <c r="U13">
-        <v>3.210965874462875</v>
+        <v>3.145207224</v>
       </c>
       <c r="V13">
-        <v>3.210965874462875</v>
+        <v>3.145207224</v>
       </c>
       <c r="W13">
-        <v>3.210965874462875</v>
+        <v>3.145207224</v>
       </c>
       <c r="X13">
-        <v>3.210965874462875</v>
+        <v>3.145207224</v>
       </c>
       <c r="Y13">
-        <v>3.210965874462875</v>
+        <v>3.145207224</v>
       </c>
       <c r="Z13">
-        <v>3.210965874462875</v>
+        <v>3.145207224</v>
       </c>
       <c r="AA13">
-        <v>3.210965874462875</v>
+        <v>3.145207224</v>
       </c>
       <c r="AB13">
-        <v>3.210965874462875</v>
+        <v>3.145207224</v>
       </c>
       <c r="AC13">
-        <v>3.210965874462875</v>
+        <v>3.145207224</v>
       </c>
       <c r="AD13">
-        <v>3.210965874462875</v>
+        <v>3.145207224</v>
       </c>
       <c r="AE13">
-        <v>3.210965874462875</v>
+        <v>3.145207224</v>
       </c>
       <c r="AF13">
-        <v>3.210965874462875</v>
+        <v>3.145207224</v>
       </c>
       <c r="AG13">
-        <v>3.210965874462875</v>
+        <v>3.145207224</v>
       </c>
       <c r="AH13">
-        <v>3.210965874462875</v>
+        <v>3.145207224</v>
       </c>
       <c r="AI13">
-        <v>3.210965874462875</v>
+        <v>3.145207224</v>
       </c>
       <c r="AJ13">
-        <v>3.210965874462875</v>
+        <v>3.145207224</v>
       </c>
       <c r="AK13">
-        <v>3.210965874462875</v>
+        <v>3.145207224</v>
       </c>
       <c r="AL13">
-        <v>3.210965874462875</v>
+        <v>3.145207224</v>
       </c>
       <c r="AM13">
-        <v>3.210965874462875</v>
+        <v>3.145207224</v>
       </c>
       <c r="AN13">
-        <v>3.210965874462875</v>
+        <v>3.145207224</v>
       </c>
       <c r="AO13">
-        <v>3.210965874462875</v>
+        <v>3.145207224</v>
       </c>
       <c r="AP13">
-        <v>3.210965874462875</v>
+        <v>3.145207224</v>
       </c>
       <c r="AQ13">
-        <v>3.210965874462875</v>
+        <v>3.145207224</v>
       </c>
       <c r="AR13">
-        <v>3.210965874462875</v>
+        <v>3.145207224</v>
       </c>
       <c r="AS13">
-        <v>3.210965874462875</v>
+        <v>3.145207224</v>
       </c>
     </row>
     <row r="14" spans="1:45">

</xml_diff>